<commit_message>
simulation update. 1 QOI
</commit_message>
<xml_diff>
--- a/QOIList.xlsx
+++ b/QOIList.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Zagreb\Downloads\Docs\Classes\Gov2001\Code\probSimulator\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F6A832FF-601E-4C38-A4AB-42F2DBE9DF61}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E589573D-A3FD-429B-ADC6-BD1A74A4D87B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{242DAC13-3634-4804-9EC3-33EBAAD95D1A}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
   <si>
     <t>FunctionName</t>
   </si>
@@ -42,16 +42,10 @@
     <t>Name</t>
   </si>
   <si>
-    <t>Probability Y &gt; k</t>
+    <t>Y for chosen X</t>
   </si>
   <si>
-    <t>probabilityGreaterThanOutputs</t>
-  </si>
-  <si>
-    <t>Y squared</t>
-  </si>
-  <si>
-    <t>ySquaredOutputs</t>
+    <t>ycOutput</t>
   </si>
 </sst>
 </file>
@@ -418,10 +412,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5C1413A3-FA11-49F9-8EC1-BE9E4A884791}">
-  <dimension ref="A1:B3"/>
+  <dimension ref="A1:B2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
+      <selection activeCell="A3" sqref="A3:XFD4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -446,14 +440,6 @@
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A3" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="B3" s="1" t="s">
-        <v>5</v>
-      </c>
-    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
tweaks and major bugfix for removing collinear X
</commit_message>
<xml_diff>
--- a/QOIList.xlsx
+++ b/QOIList.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\zagre\Documents\probSimulator\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9C7B7335-17E9-4F36-BA54-2C49757A218E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C1397773-1D0A-4FF5-9477-A52378FA50EB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{242DAC13-3634-4804-9EC3-33EBAAD95D1A}"/>
   </bookViews>
@@ -63,7 +63,7 @@
     <t>expValsOutput</t>
   </si>
   <si>
-    <t>Sim. Parameter</t>
+    <t>Sim Parameter</t>
   </si>
 </sst>
 </file>

</xml_diff>